<commit_message>
dict updates, registration bug fix and refactoring
</commit_message>
<xml_diff>
--- a/python/Dictionaries/Answers.xlsx
+++ b/python/Dictionaries/Answers.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15465" windowHeight="4830"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15465" windowHeight="4560"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="16">
   <si>
     <t>room</t>
   </si>
@@ -57,6 +57,21 @@
   </si>
   <si>
     <t>הדר צודקת ואורי טועה,אורי טועה והדר צודקת,רק הדר צודקת,הדר צודקת וגם אורי טועה,אורי טועה וגם הדר צודקת</t>
+  </si>
+  <si>
+    <t>כן</t>
+  </si>
+  <si>
+    <t>מקבילית,מקבלת,מקבלית</t>
+  </si>
+  <si>
+    <t>מלבן</t>
+  </si>
+  <si>
+    <t>אלכסונים מאונכים,אלחסונים מעונחים,אלכסונים מאונחים,מאונכים זה לזה,מאונכים,מאונכים זל"ז</t>
+  </si>
+  <si>
+    <t>מרובע סתם,מרובע כל שהוא,מרובע,מרובע בלי שם,אינשם,סתם מרובע,מרובע כלשהו</t>
   </si>
 </sst>
 </file>
@@ -93,14 +108,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -447,7 +456,7 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -458,7 +467,7 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -472,7 +481,7 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -486,7 +495,7 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -500,14 +509,1202 @@
       <c r="C6">
         <v>3</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>668</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D8" s="2"/>
+      <c r="A8">
+        <v>668</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>668</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>668</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>668</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>669</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>669</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>669</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>669</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>669</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>670</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>670</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>670</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>670</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>670</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>691</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>691</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>691</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>691</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>691</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>692</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>692</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>692</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>692</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>692</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>693</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>693</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>693</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>693</v>
+      </c>
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>693</v>
+      </c>
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>694</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>694</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>694</v>
+      </c>
+      <c r="B39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>694</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <v>5</v>
+      </c>
+      <c r="D40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>694</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+      <c r="D41" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>695</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>695</v>
+      </c>
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>695</v>
+      </c>
+      <c r="B44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>695</v>
+      </c>
+      <c r="B45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="D45" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>695</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>696</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>696</v>
+      </c>
+      <c r="B48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>696</v>
+      </c>
+      <c r="B49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
+      </c>
+      <c r="D49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>696</v>
+      </c>
+      <c r="B50" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50">
+        <v>5</v>
+      </c>
+      <c r="D50" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>696</v>
+      </c>
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+      <c r="D51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>697</v>
+      </c>
+      <c r="B52" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>697</v>
+      </c>
+      <c r="B53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>697</v>
+      </c>
+      <c r="B54" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="D54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>697</v>
+      </c>
+      <c r="B55" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
+      </c>
+      <c r="D55" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>697</v>
+      </c>
+      <c r="B56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56">
+        <v>3</v>
+      </c>
+      <c r="D56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>698</v>
+      </c>
+      <c r="B57" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="D57" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>698</v>
+      </c>
+      <c r="B58" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+      <c r="D58" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>698</v>
+      </c>
+      <c r="B59" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59">
+        <v>4</v>
+      </c>
+      <c r="D59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>698</v>
+      </c>
+      <c r="B60" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60">
+        <v>5</v>
+      </c>
+      <c r="D60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>698</v>
+      </c>
+      <c r="B61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>699</v>
+      </c>
+      <c r="B62" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>699</v>
+      </c>
+      <c r="B63" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63">
+        <v>3</v>
+      </c>
+      <c r="D63" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>699</v>
+      </c>
+      <c r="B64" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64">
+        <v>4</v>
+      </c>
+      <c r="D64" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>699</v>
+      </c>
+      <c r="B65" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65">
+        <v>5</v>
+      </c>
+      <c r="D65" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>699</v>
+      </c>
+      <c r="B66" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66">
+        <v>3</v>
+      </c>
+      <c r="D66" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>700</v>
+      </c>
+      <c r="B67" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67">
+        <v>3</v>
+      </c>
+      <c r="D67" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>700</v>
+      </c>
+      <c r="B68" t="s">
+        <v>4</v>
+      </c>
+      <c r="C68">
+        <v>3</v>
+      </c>
+      <c r="D68" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>700</v>
+      </c>
+      <c r="B69" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69">
+        <v>4</v>
+      </c>
+      <c r="D69" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>700</v>
+      </c>
+      <c r="B70" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70">
+        <v>5</v>
+      </c>
+      <c r="D70" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>700</v>
+      </c>
+      <c r="B71" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71">
+        <v>3</v>
+      </c>
+      <c r="D71" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>701</v>
+      </c>
+      <c r="B72" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72">
+        <v>3</v>
+      </c>
+      <c r="D72" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>701</v>
+      </c>
+      <c r="B73" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73">
+        <v>3</v>
+      </c>
+      <c r="D73" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>701</v>
+      </c>
+      <c r="B74" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74">
+        <v>4</v>
+      </c>
+      <c r="D74" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>701</v>
+      </c>
+      <c r="B75" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75">
+        <v>5</v>
+      </c>
+      <c r="D75" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>701</v>
+      </c>
+      <c r="B76" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76">
+        <v>3</v>
+      </c>
+      <c r="D76" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>702</v>
+      </c>
+      <c r="B77" t="s">
+        <v>3</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>702</v>
+      </c>
+      <c r="B78" t="s">
+        <v>4</v>
+      </c>
+      <c r="C78">
+        <v>3</v>
+      </c>
+      <c r="D78" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>702</v>
+      </c>
+      <c r="B79" t="s">
+        <v>4</v>
+      </c>
+      <c r="C79">
+        <v>4</v>
+      </c>
+      <c r="D79" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>702</v>
+      </c>
+      <c r="B80" t="s">
+        <v>4</v>
+      </c>
+      <c r="C80">
+        <v>5</v>
+      </c>
+      <c r="D80" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>702</v>
+      </c>
+      <c r="B81" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81">
+        <v>3</v>
+      </c>
+      <c r="D81" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>703</v>
+      </c>
+      <c r="B82" t="s">
+        <v>3</v>
+      </c>
+      <c r="C82">
+        <v>3</v>
+      </c>
+      <c r="D82" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>703</v>
+      </c>
+      <c r="B83" t="s">
+        <v>4</v>
+      </c>
+      <c r="C83">
+        <v>3</v>
+      </c>
+      <c r="D83" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>703</v>
+      </c>
+      <c r="B84" t="s">
+        <v>4</v>
+      </c>
+      <c r="C84">
+        <v>4</v>
+      </c>
+      <c r="D84" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>703</v>
+      </c>
+      <c r="B85" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85">
+        <v>5</v>
+      </c>
+      <c r="D85" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>703</v>
+      </c>
+      <c r="B86" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86">
+        <v>3</v>
+      </c>
+      <c r="D86" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>704</v>
+      </c>
+      <c r="B87" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87">
+        <v>3</v>
+      </c>
+      <c r="D87" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>704</v>
+      </c>
+      <c r="B88" t="s">
+        <v>4</v>
+      </c>
+      <c r="C88">
+        <v>3</v>
+      </c>
+      <c r="D88" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>704</v>
+      </c>
+      <c r="B89" t="s">
+        <v>4</v>
+      </c>
+      <c r="C89">
+        <v>4</v>
+      </c>
+      <c r="D89" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>704</v>
+      </c>
+      <c r="B90" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90">
+        <v>5</v>
+      </c>
+      <c r="D90" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>704</v>
+      </c>
+      <c r="B91" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91">
+        <v>3</v>
+      </c>
+      <c r="D91" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
improved correct/incorrect answers support
</commit_message>
<xml_diff>
--- a/python/Dictionaries/Answers.xlsx
+++ b/python/Dictionaries/Answers.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hindi\Source\Repos\SAGLET\python\Dictionaries\"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="27">
   <si>
     <t>room</t>
   </si>
@@ -72,6 +72,39 @@
   </si>
   <si>
     <t>מרובע סתם,מרובע כל שהוא,מרובע,מרובע בלי שם,אינשם,סתם מרובע,מרובע כלשהו</t>
+  </si>
+  <si>
+    <t>הזווית אינה יכולה להיות זווית ישרה,לעולם לא,הזווית אינה יכולה להיות בת 90 מעלות,אף פעם,לא ייתכן,בלתי אפשרי,הזוית לעולם לא תהיה זוית ישרה,הזוית אינה יכולה להיות זוית ישרה,לעולם לא,הזוית אינה יכולה להיות בת 90 מעלות,אף פעם,לא ייתכן,בלתי אפשרי,הזוית לעולם לא תהיה זוית ישרה,הזווית לא יכולה להיות ישרה,הזווית לא תהיה ישרה,הזוית לא יכולה להיות ישרה,הזווית לא תהיה ישרה</t>
+  </si>
+  <si>
+    <t>הזווית גדולה מ90 מעלות וקטנה מ180 מעלות,הזווית גדולה מ90 וקטנה מ180,הזווית גדולה מזווית ישרה וקטנה מזווית שטוחה,הזווית גדולה מ 90 מעלות וקטנה מ 180 מעלות,הזווית גדולה מ 90 וקטנה מ 180,הזוית גדולה מזווית ישרה וקטנה מזוית שטוחה,הזווית גדולה מ-90 מעלות וקטנה מ-180 מעלות,הזווית גדולה מ-90 וקטנה מ-180</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>מרובע</t>
+  </si>
+  <si>
+    <t>משולש ה'ב'ג' חופף למשולש ד'ב'א',משולש ג'ב'ה' חופף למשולש א'ב'ד,משולש ב'ג'ה' חופף למשולש ב'א'ד'</t>
+  </si>
+  <si>
+    <t>יש למקם את הנקודה על האנך האמצעי ומספר הנקודות האפשרי הוא:אינסופי,יש למקם את הנקודה על גבי האנך האמצעי ומספר הנקודות האפשרי הוא:אינסוף,יש למקם את הנקודה על האנך האמצעי ומספר הנקודות האפשרי הוא: אינסופי,יש למקם את הנקודה על גבי האנך האמצעי ומספר הנקודות האפשרי הוא: אינסוף</t>
+  </si>
+  <si>
+    <t>המרובע הוא טרפז,המרובע הוא: טרפז,המרובע הוא:טרפז</t>
   </si>
 </sst>
 </file>
@@ -108,8 +141,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,14 +460,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="3" width="9" style="1"/>
     <col min="4" max="4" width="120.625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -439,10 +476,10 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D1" t="s">
@@ -453,7 +490,7 @@
       <c r="A2">
         <v>666</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
@@ -464,7 +501,7 @@
       <c r="A3">
         <v>667</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
@@ -475,11 +512,11 @@
       <c r="A4">
         <v>667</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -489,11 +526,11 @@
       <c r="A5">
         <v>667</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -503,11 +540,11 @@
       <c r="A6">
         <v>667</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -517,11 +554,11 @@
       <c r="A7">
         <v>668</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -531,11 +568,11 @@
       <c r="A8">
         <v>668</v>
       </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -545,11 +582,11 @@
       <c r="A9">
         <v>668</v>
       </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -559,11 +596,11 @@
       <c r="A10">
         <v>668</v>
       </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D10" t="s">
         <v>14</v>
@@ -573,11 +610,11 @@
       <c r="A11">
         <v>668</v>
       </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
@@ -587,11 +624,11 @@
       <c r="A12">
         <v>669</v>
       </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -601,11 +638,11 @@
       <c r="A13">
         <v>669</v>
       </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>3</v>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
@@ -615,11 +652,11 @@
       <c r="A14">
         <v>669</v>
       </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14">
-        <v>4</v>
+      <c r="B14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
@@ -629,11 +666,11 @@
       <c r="A15">
         <v>669</v>
       </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <v>5</v>
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
@@ -643,11 +680,11 @@
       <c r="A16">
         <v>669</v>
       </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
@@ -657,11 +694,11 @@
       <c r="A17">
         <v>670</v>
       </c>
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17">
-        <v>3</v>
+      <c r="B17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
@@ -671,11 +708,11 @@
       <c r="A18">
         <v>670</v>
       </c>
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
+      <c r="B18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D18" t="s">
         <v>13</v>
@@ -685,11 +722,11 @@
       <c r="A19">
         <v>670</v>
       </c>
-      <c r="B19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19">
-        <v>4</v>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -699,11 +736,11 @@
       <c r="A20">
         <v>670</v>
       </c>
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20">
-        <v>5</v>
+      <c r="B20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D20" t="s">
         <v>14</v>
@@ -713,11 +750,11 @@
       <c r="A21">
         <v>670</v>
       </c>
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
+      <c r="B21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
@@ -727,11 +764,11 @@
       <c r="A22">
         <v>691</v>
       </c>
-      <c r="B22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22">
-        <v>3</v>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
@@ -741,11 +778,11 @@
       <c r="A23">
         <v>691</v>
       </c>
-      <c r="B23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23">
-        <v>3</v>
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D23" t="s">
         <v>13</v>
@@ -755,11 +792,11 @@
       <c r="A24">
         <v>691</v>
       </c>
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24">
-        <v>4</v>
+      <c r="B24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -769,11 +806,11 @@
       <c r="A25">
         <v>691</v>
       </c>
-      <c r="B25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25">
-        <v>5</v>
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D25" t="s">
         <v>14</v>
@@ -783,11 +820,11 @@
       <c r="A26">
         <v>691</v>
       </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26">
-        <v>3</v>
+      <c r="B26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D26" t="s">
         <v>15</v>
@@ -797,11 +834,11 @@
       <c r="A27">
         <v>692</v>
       </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27">
-        <v>3</v>
+      <c r="B27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
@@ -811,11 +848,11 @@
       <c r="A28">
         <v>692</v>
       </c>
-      <c r="B28" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28">
-        <v>3</v>
+      <c r="B28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D28" t="s">
         <v>13</v>
@@ -825,11 +862,11 @@
       <c r="A29">
         <v>692</v>
       </c>
-      <c r="B29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29">
-        <v>4</v>
+      <c r="B29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -839,11 +876,11 @@
       <c r="A30">
         <v>692</v>
       </c>
-      <c r="B30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30">
-        <v>5</v>
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D30" t="s">
         <v>14</v>
@@ -853,11 +890,11 @@
       <c r="A31">
         <v>692</v>
       </c>
-      <c r="B31" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31">
-        <v>3</v>
+      <c r="B31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D31" t="s">
         <v>15</v>
@@ -867,11 +904,11 @@
       <c r="A32">
         <v>693</v>
       </c>
-      <c r="B32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32">
-        <v>3</v>
+      <c r="B32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
@@ -881,11 +918,11 @@
       <c r="A33">
         <v>693</v>
       </c>
-      <c r="B33" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33">
-        <v>3</v>
+      <c r="B33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D33" t="s">
         <v>13</v>
@@ -895,11 +932,11 @@
       <c r="A34">
         <v>693</v>
       </c>
-      <c r="B34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34">
-        <v>4</v>
+      <c r="B34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
@@ -909,11 +946,11 @@
       <c r="A35">
         <v>693</v>
       </c>
-      <c r="B35" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35">
-        <v>5</v>
+      <c r="B35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D35" t="s">
         <v>14</v>
@@ -923,11 +960,11 @@
       <c r="A36">
         <v>693</v>
       </c>
-      <c r="B36" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36">
-        <v>3</v>
+      <c r="B36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D36" t="s">
         <v>15</v>
@@ -937,11 +974,11 @@
       <c r="A37">
         <v>694</v>
       </c>
-      <c r="B37" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37">
-        <v>3</v>
+      <c r="B37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D37" t="s">
         <v>12</v>
@@ -951,11 +988,11 @@
       <c r="A38">
         <v>694</v>
       </c>
-      <c r="B38" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38">
-        <v>3</v>
+      <c r="B38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D38" t="s">
         <v>13</v>
@@ -965,11 +1002,11 @@
       <c r="A39">
         <v>694</v>
       </c>
-      <c r="B39" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39">
-        <v>4</v>
+      <c r="B39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
@@ -979,11 +1016,11 @@
       <c r="A40">
         <v>694</v>
       </c>
-      <c r="B40" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40">
-        <v>5</v>
+      <c r="B40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D40" t="s">
         <v>14</v>
@@ -993,11 +1030,11 @@
       <c r="A41">
         <v>694</v>
       </c>
-      <c r="B41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41">
-        <v>3</v>
+      <c r="B41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D41" t="s">
         <v>15</v>
@@ -1007,11 +1044,11 @@
       <c r="A42">
         <v>695</v>
       </c>
-      <c r="B42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42">
-        <v>3</v>
+      <c r="B42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
@@ -1021,11 +1058,11 @@
       <c r="A43">
         <v>695</v>
       </c>
-      <c r="B43" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43">
-        <v>3</v>
+      <c r="B43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D43" t="s">
         <v>13</v>
@@ -1035,11 +1072,11 @@
       <c r="A44">
         <v>695</v>
       </c>
-      <c r="B44" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44">
-        <v>4</v>
+      <c r="B44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -1049,11 +1086,11 @@
       <c r="A45">
         <v>695</v>
       </c>
-      <c r="B45" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45">
-        <v>5</v>
+      <c r="B45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D45" t="s">
         <v>14</v>
@@ -1063,11 +1100,11 @@
       <c r="A46">
         <v>695</v>
       </c>
-      <c r="B46" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46">
-        <v>3</v>
+      <c r="B46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D46" t="s">
         <v>15</v>
@@ -1077,11 +1114,11 @@
       <c r="A47">
         <v>696</v>
       </c>
-      <c r="B47" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47">
-        <v>3</v>
+      <c r="B47" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D47" t="s">
         <v>12</v>
@@ -1091,11 +1128,11 @@
       <c r="A48">
         <v>696</v>
       </c>
-      <c r="B48" t="s">
-        <v>4</v>
-      </c>
-      <c r="C48">
-        <v>3</v>
+      <c r="B48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D48" t="s">
         <v>13</v>
@@ -1105,11 +1142,11 @@
       <c r="A49">
         <v>696</v>
       </c>
-      <c r="B49" t="s">
-        <v>4</v>
-      </c>
-      <c r="C49">
-        <v>4</v>
+      <c r="B49" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
@@ -1119,11 +1156,11 @@
       <c r="A50">
         <v>696</v>
       </c>
-      <c r="B50" t="s">
-        <v>4</v>
-      </c>
-      <c r="C50">
-        <v>5</v>
+      <c r="B50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D50" t="s">
         <v>14</v>
@@ -1133,11 +1170,11 @@
       <c r="A51">
         <v>696</v>
       </c>
-      <c r="B51" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51">
-        <v>3</v>
+      <c r="B51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D51" t="s">
         <v>15</v>
@@ -1147,11 +1184,11 @@
       <c r="A52">
         <v>697</v>
       </c>
-      <c r="B52" t="s">
-        <v>3</v>
-      </c>
-      <c r="C52">
-        <v>3</v>
+      <c r="B52" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
@@ -1161,11 +1198,11 @@
       <c r="A53">
         <v>697</v>
       </c>
-      <c r="B53" t="s">
-        <v>4</v>
-      </c>
-      <c r="C53">
-        <v>3</v>
+      <c r="B53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D53" t="s">
         <v>13</v>
@@ -1175,11 +1212,11 @@
       <c r="A54">
         <v>697</v>
       </c>
-      <c r="B54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C54">
-        <v>4</v>
+      <c r="B54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D54" t="s">
         <v>11</v>
@@ -1189,11 +1226,11 @@
       <c r="A55">
         <v>697</v>
       </c>
-      <c r="B55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C55">
-        <v>5</v>
+      <c r="B55" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D55" t="s">
         <v>14</v>
@@ -1203,11 +1240,11 @@
       <c r="A56">
         <v>697</v>
       </c>
-      <c r="B56" t="s">
-        <v>5</v>
-      </c>
-      <c r="C56">
-        <v>3</v>
+      <c r="B56" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D56" t="s">
         <v>15</v>
@@ -1217,11 +1254,11 @@
       <c r="A57">
         <v>698</v>
       </c>
-      <c r="B57" t="s">
-        <v>3</v>
-      </c>
-      <c r="C57">
-        <v>3</v>
+      <c r="B57" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D57" t="s">
         <v>12</v>
@@ -1231,11 +1268,11 @@
       <c r="A58">
         <v>698</v>
       </c>
-      <c r="B58" t="s">
-        <v>4</v>
-      </c>
-      <c r="C58">
-        <v>3</v>
+      <c r="B58" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D58" t="s">
         <v>13</v>
@@ -1245,11 +1282,11 @@
       <c r="A59">
         <v>698</v>
       </c>
-      <c r="B59" t="s">
-        <v>4</v>
-      </c>
-      <c r="C59">
-        <v>4</v>
+      <c r="B59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D59" t="s">
         <v>11</v>
@@ -1259,11 +1296,11 @@
       <c r="A60">
         <v>698</v>
       </c>
-      <c r="B60" t="s">
-        <v>4</v>
-      </c>
-      <c r="C60">
-        <v>5</v>
+      <c r="B60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D60" t="s">
         <v>14</v>
@@ -1273,11 +1310,11 @@
       <c r="A61">
         <v>698</v>
       </c>
-      <c r="B61" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61">
-        <v>3</v>
+      <c r="B61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D61" t="s">
         <v>15</v>
@@ -1287,11 +1324,11 @@
       <c r="A62">
         <v>699</v>
       </c>
-      <c r="B62" t="s">
-        <v>3</v>
-      </c>
-      <c r="C62">
-        <v>3</v>
+      <c r="B62" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D62" t="s">
         <v>12</v>
@@ -1301,11 +1338,11 @@
       <c r="A63">
         <v>699</v>
       </c>
-      <c r="B63" t="s">
-        <v>4</v>
-      </c>
-      <c r="C63">
-        <v>3</v>
+      <c r="B63" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D63" t="s">
         <v>13</v>
@@ -1315,11 +1352,11 @@
       <c r="A64">
         <v>699</v>
       </c>
-      <c r="B64" t="s">
-        <v>4</v>
-      </c>
-      <c r="C64">
-        <v>4</v>
+      <c r="B64" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D64" t="s">
         <v>11</v>
@@ -1329,11 +1366,11 @@
       <c r="A65">
         <v>699</v>
       </c>
-      <c r="B65" t="s">
-        <v>4</v>
-      </c>
-      <c r="C65">
-        <v>5</v>
+      <c r="B65" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D65" t="s">
         <v>14</v>
@@ -1343,11 +1380,11 @@
       <c r="A66">
         <v>699</v>
       </c>
-      <c r="B66" t="s">
-        <v>5</v>
-      </c>
-      <c r="C66">
-        <v>3</v>
+      <c r="B66" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D66" t="s">
         <v>15</v>
@@ -1357,11 +1394,11 @@
       <c r="A67">
         <v>700</v>
       </c>
-      <c r="B67" t="s">
-        <v>3</v>
-      </c>
-      <c r="C67">
-        <v>3</v>
+      <c r="B67" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D67" t="s">
         <v>12</v>
@@ -1371,11 +1408,11 @@
       <c r="A68">
         <v>700</v>
       </c>
-      <c r="B68" t="s">
-        <v>4</v>
-      </c>
-      <c r="C68">
-        <v>3</v>
+      <c r="B68" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D68" t="s">
         <v>13</v>
@@ -1385,11 +1422,11 @@
       <c r="A69">
         <v>700</v>
       </c>
-      <c r="B69" t="s">
-        <v>4</v>
-      </c>
-      <c r="C69">
-        <v>4</v>
+      <c r="B69" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D69" t="s">
         <v>11</v>
@@ -1399,11 +1436,11 @@
       <c r="A70">
         <v>700</v>
       </c>
-      <c r="B70" t="s">
-        <v>4</v>
-      </c>
-      <c r="C70">
-        <v>5</v>
+      <c r="B70" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D70" t="s">
         <v>14</v>
@@ -1413,11 +1450,11 @@
       <c r="A71">
         <v>700</v>
       </c>
-      <c r="B71" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71">
-        <v>3</v>
+      <c r="B71" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D71" t="s">
         <v>15</v>
@@ -1427,11 +1464,11 @@
       <c r="A72">
         <v>701</v>
       </c>
-      <c r="B72" t="s">
-        <v>3</v>
-      </c>
-      <c r="C72">
-        <v>3</v>
+      <c r="B72" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D72" t="s">
         <v>12</v>
@@ -1441,11 +1478,11 @@
       <c r="A73">
         <v>701</v>
       </c>
-      <c r="B73" t="s">
-        <v>4</v>
-      </c>
-      <c r="C73">
-        <v>3</v>
+      <c r="B73" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D73" t="s">
         <v>13</v>
@@ -1455,11 +1492,11 @@
       <c r="A74">
         <v>701</v>
       </c>
-      <c r="B74" t="s">
-        <v>4</v>
-      </c>
-      <c r="C74">
-        <v>4</v>
+      <c r="B74" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D74" t="s">
         <v>11</v>
@@ -1469,11 +1506,11 @@
       <c r="A75">
         <v>701</v>
       </c>
-      <c r="B75" t="s">
-        <v>4</v>
-      </c>
-      <c r="C75">
-        <v>5</v>
+      <c r="B75" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D75" t="s">
         <v>14</v>
@@ -1483,11 +1520,11 @@
       <c r="A76">
         <v>701</v>
       </c>
-      <c r="B76" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76">
-        <v>3</v>
+      <c r="B76" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D76" t="s">
         <v>15</v>
@@ -1497,11 +1534,11 @@
       <c r="A77">
         <v>702</v>
       </c>
-      <c r="B77" t="s">
-        <v>3</v>
-      </c>
-      <c r="C77">
-        <v>3</v>
+      <c r="B77" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D77" t="s">
         <v>12</v>
@@ -1511,11 +1548,11 @@
       <c r="A78">
         <v>702</v>
       </c>
-      <c r="B78" t="s">
-        <v>4</v>
-      </c>
-      <c r="C78">
-        <v>3</v>
+      <c r="B78" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D78" t="s">
         <v>13</v>
@@ -1525,11 +1562,11 @@
       <c r="A79">
         <v>702</v>
       </c>
-      <c r="B79" t="s">
-        <v>4</v>
-      </c>
-      <c r="C79">
-        <v>4</v>
+      <c r="B79" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D79" t="s">
         <v>11</v>
@@ -1539,11 +1576,11 @@
       <c r="A80">
         <v>702</v>
       </c>
-      <c r="B80" t="s">
-        <v>4</v>
-      </c>
-      <c r="C80">
-        <v>5</v>
+      <c r="B80" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D80" t="s">
         <v>14</v>
@@ -1553,11 +1590,11 @@
       <c r="A81">
         <v>702</v>
       </c>
-      <c r="B81" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81">
-        <v>3</v>
+      <c r="B81" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D81" t="s">
         <v>15</v>
@@ -1567,11 +1604,11 @@
       <c r="A82">
         <v>703</v>
       </c>
-      <c r="B82" t="s">
-        <v>3</v>
-      </c>
-      <c r="C82">
-        <v>3</v>
+      <c r="B82" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D82" t="s">
         <v>12</v>
@@ -1581,11 +1618,11 @@
       <c r="A83">
         <v>703</v>
       </c>
-      <c r="B83" t="s">
-        <v>4</v>
-      </c>
-      <c r="C83">
-        <v>3</v>
+      <c r="B83" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D83" t="s">
         <v>13</v>
@@ -1595,11 +1632,11 @@
       <c r="A84">
         <v>703</v>
       </c>
-      <c r="B84" t="s">
-        <v>4</v>
-      </c>
-      <c r="C84">
-        <v>4</v>
+      <c r="B84" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D84" t="s">
         <v>11</v>
@@ -1609,11 +1646,11 @@
       <c r="A85">
         <v>703</v>
       </c>
-      <c r="B85" t="s">
-        <v>4</v>
-      </c>
-      <c r="C85">
-        <v>5</v>
+      <c r="B85" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D85" t="s">
         <v>14</v>
@@ -1623,11 +1660,11 @@
       <c r="A86">
         <v>703</v>
       </c>
-      <c r="B86" t="s">
-        <v>5</v>
-      </c>
-      <c r="C86">
-        <v>3</v>
+      <c r="B86" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D86" t="s">
         <v>15</v>
@@ -1637,11 +1674,11 @@
       <c r="A87">
         <v>704</v>
       </c>
-      <c r="B87" t="s">
-        <v>3</v>
-      </c>
-      <c r="C87">
-        <v>3</v>
+      <c r="B87" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D87" t="s">
         <v>12</v>
@@ -1651,11 +1688,11 @@
       <c r="A88">
         <v>704</v>
       </c>
-      <c r="B88" t="s">
-        <v>4</v>
-      </c>
-      <c r="C88">
-        <v>3</v>
+      <c r="B88" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D88" t="s">
         <v>13</v>
@@ -1665,11 +1702,11 @@
       <c r="A89">
         <v>704</v>
       </c>
-      <c r="B89" t="s">
-        <v>4</v>
-      </c>
-      <c r="C89">
-        <v>4</v>
+      <c r="B89" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D89" t="s">
         <v>11</v>
@@ -1679,11 +1716,11 @@
       <c r="A90">
         <v>704</v>
       </c>
-      <c r="B90" t="s">
-        <v>4</v>
-      </c>
-      <c r="C90">
-        <v>5</v>
+      <c r="B90" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D90" t="s">
         <v>14</v>
@@ -1693,14 +1730,322 @@
       <c r="A91">
         <v>704</v>
       </c>
-      <c r="B91" t="s">
-        <v>5</v>
-      </c>
-      <c r="C91">
-        <v>3</v>
+      <c r="B91" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D91" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>716</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D92" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>716</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D93" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>717</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D94" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>717</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D95" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>718</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D96" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>718</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D97" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>719</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D98" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>719</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D99" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>720</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D100" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>720</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D101" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>728</v>
+      </c>
+      <c r="B102" t="s">
+        <v>3</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D102" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>729</v>
+      </c>
+      <c r="B103" t="s">
+        <v>3</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D103" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>730</v>
+      </c>
+      <c r="B104" t="s">
+        <v>3</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D104" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>731</v>
+      </c>
+      <c r="B105" t="s">
+        <v>3</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D105" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>732</v>
+      </c>
+      <c r="B106" t="s">
+        <v>4</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D106" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>732</v>
+      </c>
+      <c r="B107" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D107" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>733</v>
+      </c>
+      <c r="B108" t="s">
+        <v>4</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D108" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>733</v>
+      </c>
+      <c r="B109" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D109" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>734</v>
+      </c>
+      <c r="B110" t="s">
+        <v>4</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D110" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>734</v>
+      </c>
+      <c r="B111" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D111" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>735</v>
+      </c>
+      <c r="B112" t="s">
+        <v>4</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D112" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>735</v>
+      </c>
+      <c r="B113" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D113" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
blocking communication (much lower memory usage)
</commit_message>
<xml_diff>
--- a/python/Dictionaries/Answers.xlsx
+++ b/python/Dictionaries/Answers.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="30">
   <si>
     <t>room</t>
   </si>
@@ -105,6 +105,15 @@
   </si>
   <si>
     <t>המרובע הוא טרפז,המרובע הוא: טרפז,המרובע הוא:טרפז</t>
+  </si>
+  <si>
+    <t>דני צודק,צודק,צדק,כן,נכון</t>
+  </si>
+  <si>
+    <t>מיכל צודקת,כן,צודק,נכון</t>
+  </si>
+  <si>
+    <t>דני לא צודק,דני טועה,טעות,לא,טואה,תואה,תאות,לא צודק,לא נכון,דני שוגה</t>
   </si>
 </sst>
 </file>
@@ -460,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:D146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D143" sqref="D143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2048,6 +2057,369 @@
         <v>26</v>
       </c>
     </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>792</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D114" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>792</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D115" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>792</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D116" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>793</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D117" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>793</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D118" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>793</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D119" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>794</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D120" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>794</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D121" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>794</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D122" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>795</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D123" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>795</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D124" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>795</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D125" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>796</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D126" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>796</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D127" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>796</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D128" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>797</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D129" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>797</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D130" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>797</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D131" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>798</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D132" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>798</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D133" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>798</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D134" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>799</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D135" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>799</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D136" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>799</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D137" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>800</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D138" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>800</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D139" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>800</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D140" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>801</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D141" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>801</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D142" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>801</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D143" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>802</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D144" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>802</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D145" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>802</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D146" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>